<commit_message>
Added Test Report and updated Plan
Updated test plan schedule and added PDF for Test Report Summary
</commit_message>
<xml_diff>
--- a/Test Plan - Team Pluto.xlsx
+++ b/Test Plan - Team Pluto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishqp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10514E64-3B5B-492A-929A-903D19D71744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F596DC-401B-44E7-BDF9-9CBDC2CBDFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Ideas" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1507,7 +1507,7 @@
       <name val="&quot;Aptos Narrow&quot;, sans-serif"/>
     </font>
   </fonts>
-  <fills count="31">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1686,6 +1686,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor rgb="FF00B0F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FF00B050"/>
       </patternFill>
     </fill>
   </fills>
@@ -1933,7 +1951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2260,28 +2278,16 @@
     <xf numFmtId="0" fontId="27" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="30" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2318,6 +2324,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2725,7 +2749,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="14.25">
       <c r="A17" s="4" t="s">
         <v>34</v>
       </c>
@@ -2734,7 +2758,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="14.25">
       <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
@@ -2742,7 +2766,7 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="12.75">
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -2840,7 +2864,7 @@
     <col min="7" max="7" width="114.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="14.25">
       <c r="A1" s="12" t="s">
         <v>46</v>
       </c>
@@ -2949,7 +2973,7 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="14.25">
       <c r="A6" s="18" t="s">
         <v>70</v>
       </c>
@@ -2972,7 +2996,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="14.25">
       <c r="A7" s="18" t="s">
         <v>77</v>
       </c>
@@ -2995,7 +3019,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="14.25">
       <c r="A8" s="18" t="s">
         <v>84</v>
       </c>
@@ -3018,7 +3042,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="14.25">
       <c r="A9" s="18" t="s">
         <v>91</v>
       </c>
@@ -3039,7 +3063,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="14.25">
       <c r="A10" s="18" t="s">
         <v>97</v>
       </c>
@@ -3052,7 +3076,7 @@
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="14.25">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -3065,7 +3089,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="14.25">
       <c r="A12" s="19" t="s">
         <v>70</v>
       </c>
@@ -3088,7 +3112,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="14.25">
       <c r="A13" s="19" t="s">
         <v>77</v>
       </c>
@@ -3109,7 +3133,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="14.25">
       <c r="A14" s="19" t="s">
         <v>107</v>
       </c>
@@ -3132,7 +3156,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" ht="14.25">
       <c r="A15" s="19" t="s">
         <v>114</v>
       </c>
@@ -3153,7 +3177,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" ht="14.25">
       <c r="A16" s="19" t="s">
         <v>120</v>
       </c>
@@ -3174,7 +3198,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" ht="14.25">
       <c r="A17" s="20"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
@@ -3187,7 +3211,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" ht="14.25">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
@@ -61516,8 +61540,8 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -61585,7 +61609,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="141" t="s">
+      <c r="A3" s="137" t="s">
         <v>265</v>
       </c>
       <c r="B3" s="37" t="s">
@@ -61611,7 +61635,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="142"/>
+      <c r="A4" s="138"/>
       <c r="B4" s="40" t="s">
         <v>63</v>
       </c>
@@ -61631,7 +61655,7 @@
       <c r="H4" s="44"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="143"/>
+      <c r="A5" s="139"/>
       <c r="B5" s="45" t="s">
         <v>61</v>
       </c>
@@ -61647,7 +61671,7 @@
       <c r="H5" s="49"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="144" t="s">
+      <c r="A6" s="140" t="s">
         <v>268</v>
       </c>
       <c r="B6" s="50" t="s">
@@ -61673,7 +61697,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="142"/>
+      <c r="A7" s="138"/>
       <c r="B7" s="53" t="s">
         <v>270</v>
       </c>
@@ -61697,7 +61721,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="142"/>
+      <c r="A8" s="138"/>
       <c r="B8" s="56" t="s">
         <v>275</v>
       </c>
@@ -61721,7 +61745,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="142"/>
+      <c r="A9" s="138"/>
       <c r="B9" s="53" t="s">
         <v>77</v>
       </c>
@@ -61743,7 +61767,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="142"/>
+      <c r="A10" s="138"/>
       <c r="B10" s="58" t="s">
         <v>285</v>
       </c>
@@ -61761,7 +61785,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="143"/>
+      <c r="A11" s="139"/>
       <c r="B11" s="56" t="s">
         <v>97</v>
       </c>
@@ -61775,7 +61799,7 @@
       <c r="H11" s="51"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="145" t="s">
+      <c r="A12" s="141" t="s">
         <v>289</v>
       </c>
       <c r="B12" s="61" t="s">
@@ -61801,7 +61825,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="142"/>
+      <c r="A13" s="138"/>
       <c r="B13" s="63" t="s">
         <v>290</v>
       </c>
@@ -61825,7 +61849,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="142"/>
+      <c r="A14" s="138"/>
       <c r="B14" s="67" t="s">
         <v>292</v>
       </c>
@@ -61849,7 +61873,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="142"/>
+      <c r="A15" s="138"/>
       <c r="B15" s="63" t="s">
         <v>299</v>
       </c>
@@ -61871,7 +61895,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="142"/>
+      <c r="A16" s="138"/>
       <c r="B16" s="70" t="s">
         <v>120</v>
       </c>
@@ -61893,7 +61917,7 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="146" t="s">
+      <c r="A17" s="142" t="s">
         <v>306</v>
       </c>
       <c r="B17" s="72" t="s">
@@ -61919,7 +61943,7 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="147"/>
+      <c r="A18" s="143"/>
       <c r="B18" s="72"/>
       <c r="C18" s="73" t="s">
         <v>140</v>
@@ -61935,7 +61959,7 @@
       <c r="H18" s="74"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="147"/>
+      <c r="A19" s="143"/>
       <c r="B19" s="72"/>
       <c r="C19" s="72" t="s">
         <v>64</v>
@@ -61947,7 +61971,7 @@
       <c r="H19" s="74"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="147"/>
+      <c r="A20" s="143"/>
       <c r="B20" s="72"/>
       <c r="C20" s="72"/>
       <c r="D20" s="72"/>
@@ -61957,7 +61981,7 @@
       <c r="H20" s="74"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="147"/>
+      <c r="A21" s="143"/>
       <c r="B21" s="72"/>
       <c r="C21" s="72"/>
       <c r="D21" s="72"/>
@@ -62004,15 +62028,15 @@
       <c r="A1" s="75" t="s">
         <v>308</v>
       </c>
-      <c r="B1" s="148" t="s">
+      <c r="B1" s="144" t="s">
         <v>309</v>
       </c>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
     </row>
     <row r="2" spans="1:8" ht="123" customHeight="1">
       <c r="A2" s="76">
@@ -62194,7 +62218,7 @@
   </sheetPr>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -62204,7 +62228,7 @@
     <col min="2" max="2" width="113.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" ht="15">
       <c r="A1" s="92" t="s">
         <v>349</v>
       </c>
@@ -62512,7 +62536,9 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -62543,10 +62569,10 @@
       <c r="B2" s="125" t="s">
         <v>374</v>
       </c>
-      <c r="C2" s="126" t="s">
+      <c r="C2" s="151" t="s">
         <v>374</v>
       </c>
-      <c r="D2" s="127" t="s">
+      <c r="D2" s="126" t="s">
         <v>375</v>
       </c>
     </row>
@@ -62557,55 +62583,55 @@
       <c r="B3" s="125" t="s">
         <v>377</v>
       </c>
-      <c r="C3" s="126" t="s">
+      <c r="C3" s="151" t="s">
         <v>377</v>
       </c>
-      <c r="D3" s="128" t="s">
+      <c r="D3" s="127" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A4" s="129" t="s">
+      <c r="A4" s="146" t="s">
         <v>379</v>
       </c>
-      <c r="B4" s="130" t="s">
+      <c r="B4" s="147" t="s">
         <v>380</v>
       </c>
-      <c r="C4" s="130"/>
-      <c r="D4" s="131" t="s">
+      <c r="C4" s="147"/>
+      <c r="D4" s="128" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A5" s="129" t="s">
+      <c r="A5" s="149" t="s">
         <v>382</v>
       </c>
-      <c r="B5" s="130" t="s">
+      <c r="B5" s="150" t="s">
         <v>380</v>
       </c>
-      <c r="C5" s="130"/>
-      <c r="D5" s="132" t="s">
+      <c r="C5" s="150"/>
+      <c r="D5" s="129" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="129" t="s">
+    <row r="6" spans="1:4" ht="14.25">
+      <c r="A6" s="146" t="s">
         <v>384</v>
       </c>
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="147" t="s">
         <v>385</v>
       </c>
-      <c r="C6" s="133"/>
+      <c r="C6" s="148"/>
       <c r="D6" s="20"/>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="129" t="s">
+    <row r="7" spans="1:4" ht="14.25">
+      <c r="A7" s="146" t="s">
         <v>386</v>
       </c>
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="147" t="s">
         <v>385</v>
       </c>
-      <c r="C7" s="133"/>
+      <c r="C7" s="148"/>
       <c r="D7" s="20"/>
     </row>
   </sheetData>
@@ -62631,41 +62657,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="130" t="s">
         <v>387</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="131" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="136" t="s">
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="132" t="s">
         <v>389</v>
       </c>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="133" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="138" t="s">
+    <row r="3" spans="1:2" ht="14.25">
+      <c r="A3" s="134" t="s">
         <v>391</v>
       </c>
-      <c r="B3" s="139"/>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="138" t="s">
+      <c r="B3" s="135"/>
+    </row>
+    <row r="4" spans="1:2" ht="14.25">
+      <c r="A4" s="134" t="s">
         <v>392</v>
       </c>
       <c r="B4" s="20"/>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="138" t="s">
+    <row r="5" spans="1:2" ht="14.25">
+      <c r="A5" s="134" t="s">
         <v>393</v>
       </c>
       <c r="B5" s="20"/>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="140" t="s">
+    <row r="6" spans="1:2" ht="14.25">
+      <c r="A6" s="136" t="s">
         <v>394</v>
       </c>
     </row>

</xml_diff>